<commit_message>
July 3 update of en-route ATFM delay file
</commit_message>
<xml_diff>
--- a/static/download/2022/RP3_ERT_ATFM_2022_Jan_Dec.xlsx
+++ b/static/download/2022/RP3_ERT_ATFM_2022_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="161">
   <si>
     <t>Data source</t>
   </si>
@@ -486,6 +486,18 @@
   </si>
   <si>
     <t>UK removed from SES area</t>
+  </si>
+  <si>
+    <t>ENAIRE,DSNA</t>
+  </si>
+  <si>
+    <t>55 min.  of regulation 'T21316E'  (16/09/2022) reallocated from ENAIRE to DSNA</t>
+  </si>
+  <si>
+    <t>274 min.  of regulation ‘PAU23M’ (23/12/2022) reallocated from ENAIRE to DSNA</t>
+  </si>
+  <si>
+    <t>17 min. of regulation ‘LPAU23’ (23/12/2022) reallocated from ENAIRE to DSNA</t>
   </si>
 </sst>
 </file>
@@ -832,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1141,17 +1153,14 @@
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1231,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="10">
-        <v>45072.0</v>
+        <v>45110.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -1615,7 +1624,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45072</v>
+        <v>45110</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -2990,7 +2999,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45072</v>
+        <v>45110</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -3167,11 +3176,11 @@
         <v>5232079.0</v>
       </c>
       <c r="D12" s="97">
-        <v>1.0466578E7</v>
+        <v>1.0466924E7</v>
       </c>
       <c r="E12" s="96">
         <f t="shared" si="1"/>
-        <v>2.000462531</v>
+        <v>2.000528662</v>
       </c>
       <c r="F12" s="96"/>
     </row>
@@ -3201,11 +3210,11 @@
         <v>2047921.0</v>
       </c>
       <c r="D14" s="97">
-        <v>1002659.0</v>
+        <v>1002313.0</v>
       </c>
       <c r="E14" s="96">
         <f t="shared" si="1"/>
-        <v>0.4895984757</v>
+        <v>0.4894295239</v>
       </c>
       <c r="F14" s="96"/>
     </row>
@@ -3275,7 +3284,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45072</v>
+        <v>45110</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -3482,11 +3491,11 @@
         <v>2919041.0</v>
       </c>
       <c r="D13" s="97">
-        <v>4342492.0</v>
+        <v>4342838.0</v>
       </c>
       <c r="E13" s="99">
         <f t="shared" si="1"/>
-        <v>1.487643373</v>
+        <v>1.487761905</v>
       </c>
       <c r="F13" s="96"/>
     </row>
@@ -3520,11 +3529,11 @@
         <v>1982636.0</v>
       </c>
       <c r="D15" s="97">
-        <v>598463.0</v>
+        <v>598117.0</v>
       </c>
       <c r="E15" s="99">
         <f t="shared" si="1"/>
-        <v>0.3018521806</v>
+        <v>0.3016776655</v>
       </c>
       <c r="F15" s="96"/>
     </row>
@@ -3894,7 +3903,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.25"/>
-    <col customWidth="1" min="2" max="2" width="5.5"/>
+    <col customWidth="1" min="2" max="2" width="11.0"/>
     <col customWidth="1" min="3" max="3" width="11.25"/>
     <col customWidth="1" min="4" max="4" width="123.13"/>
   </cols>
@@ -3926,22 +3935,46 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="104"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="102"/>
+      <c r="A3" s="101">
+        <v>45107.0</v>
+      </c>
+      <c r="B3" s="102" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="104">
+        <v>2022.0</v>
+      </c>
+      <c r="D3" s="102" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="104"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="102"/>
+      <c r="A4" s="101">
+        <v>45107.0</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="105">
+        <v>2022.0</v>
+      </c>
+      <c r="D4" s="102" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="101"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="107"/>
+      <c r="A5" s="101">
+        <v>45107.0</v>
+      </c>
+      <c r="B5" s="106" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="104">
+        <v>2022.0</v>
+      </c>
+      <c r="D5" s="106" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
correction post ops ENAIRE
</commit_message>
<xml_diff>
--- a/static/download/2022/RP3_ERT_ATFM_2022_Jan_Dec.xlsx
+++ b/static/download/2022/RP3_ERT_ATFM_2022_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="164">
   <si>
     <t>Data source</t>
   </si>
@@ -498,6 +498,15 @@
   </si>
   <si>
     <t>17 min. of regulation ‘LPAU23’ (23/12/2022) reallocated from ENAIRE to DSNA</t>
+  </si>
+  <si>
+    <t>7878 min. of regulation 'LEROCK04' reallocated from ENAIRE to 'OTHER'</t>
+  </si>
+  <si>
+    <t>488 min. of regulation 'SAN04M' reallocated from ENAIRE to 'OTHER'</t>
+  </si>
+  <si>
+    <t>1423 min. of regulation 'SUR04M' reallocated from ENAIRE to 'OTHER'</t>
   </si>
 </sst>
 </file>
@@ -844,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="111">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1161,6 +1170,18 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1240,7 +1261,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="10">
-        <v>45110.0</v>
+        <v>45117.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -1518,20 +1539,20 @@
       </c>
       <c r="C13" s="32">
         <f t="shared" si="1"/>
-        <v>1.741019998</v>
+        <v>1.739840968</v>
       </c>
       <c r="D13" s="39">
         <v>8302587.0</v>
       </c>
       <c r="E13" s="40">
-        <v>1.445497E7</v>
+        <v>1.4445181E7</v>
       </c>
       <c r="F13" s="43">
         <v>0.5</v>
       </c>
       <c r="G13" s="42">
         <f t="shared" si="2"/>
-        <v>1.241019998</v>
+        <v>1.239840968</v>
       </c>
       <c r="H13" s="37">
         <v>0.0404</v>
@@ -1624,7 +1645,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45110</v>
+        <v>45117</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -2668,17 +2689,17 @@
       </c>
       <c r="B52" s="69">
         <f t="shared" si="1"/>
-        <v>0.4834897243</v>
+        <v>0.4676089058</v>
       </c>
       <c r="C52" s="71">
         <v>616404.0</v>
       </c>
       <c r="D52" s="71">
-        <v>298025.0</v>
+        <v>288236.0</v>
       </c>
       <c r="E52" s="69">
         <f t="shared" si="4"/>
-        <v>1.82614282</v>
+        <v>1.824869156</v>
       </c>
       <c r="F52" s="78">
         <v>1.0</v>
@@ -2700,7 +2721,7 @@
       </c>
       <c r="E53" s="69">
         <f t="shared" si="4"/>
-        <v>1.741019998</v>
+        <v>1.739840968</v>
       </c>
       <c r="F53" s="78">
         <v>1.0</v>
@@ -2999,7 +3020,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45110</v>
+        <v>45117</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -3210,11 +3231,11 @@
         <v>2047921.0</v>
       </c>
       <c r="D14" s="97">
-        <v>1002313.0</v>
+        <v>992524.0</v>
       </c>
       <c r="E14" s="96">
         <f t="shared" si="1"/>
-        <v>0.4894295239</v>
+        <v>0.4846495544</v>
       </c>
       <c r="F14" s="96"/>
     </row>
@@ -3284,7 +3305,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45110</v>
+        <v>45117</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -3529,11 +3550,11 @@
         <v>1982636.0</v>
       </c>
       <c r="D15" s="97">
-        <v>598117.0</v>
+        <v>588328.0</v>
       </c>
       <c r="E15" s="99">
         <f t="shared" si="1"/>
-        <v>0.3016776655</v>
+        <v>0.2967402993</v>
       </c>
       <c r="F15" s="96"/>
     </row>
@@ -3976,6 +3997,48 @@
         <v>160</v>
       </c>
     </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="107">
+        <v>45117.0</v>
+      </c>
+      <c r="B6" s="108" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="109">
+        <v>2022.0</v>
+      </c>
+      <c r="D6" s="108" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="110">
+        <v>45117.0</v>
+      </c>
+      <c r="B7" s="108" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="109">
+        <v>2022.0</v>
+      </c>
+      <c r="D7" s="108" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="110">
+        <v>45117.0</v>
+      </c>
+      <c r="B8" s="108" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="109">
+        <v>2022.0</v>
+      </c>
+      <c r="D8" s="108" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
post ops file updated
</commit_message>
<xml_diff>
--- a/static/download/2022/RP3_ERT_ATFM_2022_Jan_Dec.xlsx
+++ b/static/download/2022/RP3_ERT_ATFM_2022_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="166">
   <si>
     <t>Data source</t>
   </si>
@@ -507,6 +507,12 @@
   </si>
   <si>
     <t>1423 min. of regulation 'SUR04M' reallocated from ENAIRE to 'OTHER'</t>
+  </si>
+  <si>
+    <t>DFS, PANSA, ANS CR</t>
+  </si>
+  <si>
+    <t>Corrections related to impact of war in Ukraine</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1267,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="10">
-        <v>45117.0</v>
+        <v>45174.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -1539,20 +1545,20 @@
       </c>
       <c r="C13" s="32">
         <f t="shared" si="1"/>
-        <v>1.739840968</v>
+        <v>1.694278301</v>
       </c>
       <c r="D13" s="39">
         <v>8302587.0</v>
       </c>
       <c r="E13" s="40">
-        <v>1.4445181E7</v>
+        <v>1.4066893E7</v>
       </c>
       <c r="F13" s="43">
         <v>0.5</v>
       </c>
       <c r="G13" s="42">
         <f t="shared" si="2"/>
-        <v>1.239840968</v>
+        <v>1.194278301</v>
       </c>
       <c r="H13" s="37">
         <v>0.0404</v>
@@ -1645,7 +1651,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45117</v>
+        <v>45174</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -2491,17 +2497,17 @@
       </c>
       <c r="B43" s="69">
         <f t="shared" si="1"/>
-        <v>0.1812200377</v>
+        <v>0.1778860358</v>
       </c>
       <c r="C43" s="71">
         <v>463707.0</v>
       </c>
       <c r="D43" s="71">
-        <v>84033.0</v>
+        <v>82487.0</v>
       </c>
       <c r="E43" s="69">
         <f t="shared" ref="E43:E53" si="4">sum(D$42:D43)/sum(C$42:C43)</f>
-        <v>0.1734592134</v>
+        <v>0.1718175766</v>
       </c>
       <c r="F43" s="78">
         <v>1.0</v>
@@ -2513,17 +2519,17 @@
       </c>
       <c r="B44" s="69">
         <f t="shared" si="1"/>
-        <v>0.3255284979</v>
+        <v>0.2777396765</v>
       </c>
       <c r="C44" s="71">
         <v>580324.0</v>
       </c>
       <c r="D44" s="71">
-        <v>188912.0</v>
+        <v>161179.0</v>
       </c>
       <c r="E44" s="69">
         <f t="shared" si="4"/>
-        <v>0.2314392205</v>
+        <v>0.2122028794</v>
       </c>
       <c r="F44" s="78">
         <v>1.0</v>
@@ -2535,17 +2541,17 @@
       </c>
       <c r="B45" s="69">
         <f t="shared" si="1"/>
-        <v>1.396478328</v>
+        <v>1.136851254</v>
       </c>
       <c r="C45" s="71">
         <v>675361.0</v>
       </c>
       <c r="D45" s="71">
-        <v>943127.0</v>
+        <v>767785.0</v>
       </c>
       <c r="E45" s="69">
         <f t="shared" si="4"/>
-        <v>0.589504184</v>
+        <v>0.4963857746</v>
       </c>
       <c r="F45" s="78">
         <v>1.0</v>
@@ -2557,17 +2563,17 @@
       </c>
       <c r="B46" s="69">
         <f t="shared" si="1"/>
-        <v>2.074151273</v>
+        <v>1.848473429</v>
       </c>
       <c r="C46" s="71">
         <v>769535.0</v>
       </c>
       <c r="D46" s="71">
-        <v>1596132.0</v>
+        <v>1422465.0</v>
       </c>
       <c r="E46" s="69">
         <f t="shared" si="4"/>
-        <v>0.9745740004</v>
+        <v>0.8470739271</v>
       </c>
       <c r="F46" s="78">
         <v>1.0</v>
@@ -2589,7 +2595,7 @@
       </c>
       <c r="E47" s="69">
         <f t="shared" si="4"/>
-        <v>1.53673133</v>
+        <v>1.436502515</v>
       </c>
       <c r="F47" s="78">
         <v>1.0</v>
@@ -2611,7 +2617,7 @@
       </c>
       <c r="E48" s="69">
         <f t="shared" si="4"/>
-        <v>1.859164684</v>
+        <v>1.777472975</v>
       </c>
       <c r="F48" s="78">
         <v>1.0</v>
@@ -2633,7 +2639,7 @@
       </c>
       <c r="E49" s="69">
         <f t="shared" si="4"/>
-        <v>1.964167791</v>
+        <v>1.895189648</v>
       </c>
       <c r="F49" s="78">
         <v>1.0</v>
@@ -2655,7 +2661,7 @@
       </c>
       <c r="E50" s="69">
         <f t="shared" si="4"/>
-        <v>2.032147185</v>
+        <v>1.972057777</v>
       </c>
       <c r="F50" s="78">
         <v>1.0</v>
@@ -2677,7 +2683,7 @@
       </c>
       <c r="E51" s="69">
         <f t="shared" si="4"/>
-        <v>1.943214753</v>
+        <v>1.889703381</v>
       </c>
       <c r="F51" s="78">
         <v>1.0</v>
@@ -2699,7 +2705,7 @@
       </c>
       <c r="E52" s="69">
         <f t="shared" si="4"/>
-        <v>1.824869156</v>
+        <v>1.775649469</v>
       </c>
       <c r="F52" s="78">
         <v>1.0</v>
@@ -2721,7 +2727,7 @@
       </c>
       <c r="E53" s="69">
         <f t="shared" si="4"/>
-        <v>1.739840968</v>
+        <v>1.694278301</v>
       </c>
       <c r="F53" s="78">
         <v>1.0</v>
@@ -3020,7 +3026,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45117</v>
+        <v>45174</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -3092,15 +3098,15 @@
         <v>8302587.0</v>
       </c>
       <c r="D6" s="97">
-        <v>1.445497E7</v>
+        <v>1.4066893E7</v>
       </c>
       <c r="E6" s="96">
         <f t="shared" ref="E6:E15" si="1">D6/C6</f>
-        <v>1.741019998</v>
+        <v>1.694278301</v>
       </c>
       <c r="F6" s="96">
         <f>E6-B6</f>
-        <v>1.241019998</v>
+        <v>1.194278301</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -3112,11 +3118,11 @@
         <v>662296.0</v>
       </c>
       <c r="D7" s="97">
-        <v>799668.0</v>
+        <v>668941.0</v>
       </c>
       <c r="E7" s="96">
         <f t="shared" si="1"/>
-        <v>1.207417831</v>
+        <v>1.010033278</v>
       </c>
       <c r="F7" s="96"/>
     </row>
@@ -3180,11 +3186,11 @@
         <v>1943729.0</v>
       </c>
       <c r="D11" s="97">
-        <v>1767150.0</v>
+        <v>1698768.0</v>
       </c>
       <c r="E11" s="96">
         <f t="shared" si="1"/>
-        <v>0.9091545169</v>
+        <v>0.8739736867</v>
       </c>
       <c r="F11" s="96"/>
     </row>
@@ -3197,11 +3203,11 @@
         <v>5232079.0</v>
       </c>
       <c r="D12" s="97">
-        <v>1.0466924E7</v>
+        <v>1.0287745E7</v>
       </c>
       <c r="E12" s="96">
         <f t="shared" si="1"/>
-        <v>2.000528662</v>
+        <v>1.966282428</v>
       </c>
       <c r="F12" s="96"/>
     </row>
@@ -3305,7 +3311,7 @@
       </c>
       <c r="B2" s="52">
         <f>ERT_ATFM_YY!B2</f>
-        <v>45117</v>
+        <v>45174</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>6</v>
@@ -3377,11 +3383,11 @@
         <v>550194.0</v>
       </c>
       <c r="D6" s="97">
-        <v>798202.0</v>
+        <v>729820.0</v>
       </c>
       <c r="E6" s="99">
         <f t="shared" ref="E6:E33" si="1">D6/C6</f>
-        <v>1.450764639</v>
+        <v>1.32647757</v>
       </c>
       <c r="F6" s="96" t="s">
         <v>4</v>
@@ -3493,11 +3499,11 @@
         <v>2516506.0</v>
       </c>
       <c r="D12" s="97">
-        <v>5705935.0</v>
+        <v>5526756.0</v>
       </c>
       <c r="E12" s="99">
         <f t="shared" si="1"/>
-        <v>2.267403694</v>
+        <v>2.196202195</v>
       </c>
       <c r="F12" s="96"/>
     </row>
@@ -3797,11 +3803,11 @@
         <v>613073.0</v>
       </c>
       <c r="D28" s="97">
-        <v>799668.0</v>
+        <v>668941.0</v>
       </c>
       <c r="E28" s="99">
         <f t="shared" si="1"/>
-        <v>1.304360166</v>
+        <v>1.09112781</v>
       </c>
       <c r="F28" s="96"/>
     </row>
@@ -4039,6 +4045,20 @@
         <v>163</v>
       </c>
     </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="110">
+        <v>45174.0</v>
+      </c>
+      <c r="B9" s="108" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="109">
+        <v>2022.0</v>
+      </c>
+      <c r="D9" s="108" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>